<commit_message>
Correzioni e Simulation Time
</commit_message>
<xml_diff>
--- a/Documents/Calcolo Utilizzazione.xlsx
+++ b/Documents/Calcolo Utilizzazione.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5432c06226f2998e/Universita/LM-Computer Engineering/PECSN/PECSN-Project/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documenti\OneDrive\Universita\LM-Computer Engineering\PECSN\PECSN-Project\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="8_{7C6B1B4E-6765-44AE-9011-3DDA248C307B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A9DF8AE0-703A-4F6B-AFEE-0DA4B967438A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5163EB8-663E-4D21-AB85-01A993F15C9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{6CA2E0AA-0133-4EF1-B5E8-AD8D784F3B19}"/>
   </bookViews>
@@ -139,13 +139,9 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CC4E2317-C62D-4FC3-8729-E98047D0F19A}" name="Tabella1" displayName="Tabella1" ref="B3:E11" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="B3:E11" xr:uid="{CC4E2317-C62D-4FC3-8729-E98047D0F19A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CC4E2317-C62D-4FC3-8729-E98047D0F19A}" name="Tabella1" displayName="Tabella1" ref="B3:E26" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="B3:E26" xr:uid="{CC4E2317-C62D-4FC3-8729-E98047D0F19A}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{2A779C70-B05D-4564-9E37-2EFFA2AC09A3}" name="SC"/>
     <tableColumn id="2" xr3:uid="{E6C8D15D-91E3-4376-B1AA-B7E8B9822473}" name="CPU">
@@ -459,10 +455,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFB80710-4C35-42AE-97AD-C2D68AF7A1B1}">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4:L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -525,29 +521,30 @@
       </c>
       <c r="D4">
         <f>K4/H4</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E4">
         <f>L4/I4</f>
-        <v>1</v>
+        <v>13.333333333333334</v>
       </c>
       <c r="G4">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="H4">
-        <v>1</v>
+        <v>250</v>
       </c>
       <c r="I4">
-        <v>1</v>
+        <v>75</v>
       </c>
       <c r="J4">
-        <v>1</v>
+        <f>G4</f>
+        <v>1000</v>
       </c>
       <c r="K4">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="L4">
-        <v>1</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.45">
@@ -575,26 +572,26 @@
       </c>
       <c r="D6">
         <f>C6+D5*D$4</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E6">
         <f>D6+E5*E$4</f>
-        <v>3</v>
+        <v>18.333333333333336</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="G6">
-        <f t="shared" ref="G6:I11" si="0">C$4*($E5/$E6)</f>
-        <v>0.33333333333333331</v>
+        <f t="shared" ref="G6:I21" si="0">C$4*($E5/$E6)</f>
+        <v>5.4545454545454536E-2</v>
       </c>
       <c r="H6">
         <f t="shared" si="0"/>
-        <v>0.33333333333333331</v>
+        <v>0.21818181818181814</v>
       </c>
       <c r="I6">
         <f t="shared" si="0"/>
-        <v>0.33333333333333331</v>
+        <v>0.72727272727272718</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.45">
@@ -608,23 +605,23 @@
       </c>
       <c r="D7">
         <f t="shared" ref="D7:D11" si="2">C7+D6*D$4</f>
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="E7">
         <f t="shared" ref="E7:E10" si="3">D7+E6*E$4</f>
-        <v>6</v>
+        <v>265.44444444444446</v>
       </c>
       <c r="G7">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>6.9066555043951455E-2</v>
       </c>
       <c r="H7">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>0.27626622017580582</v>
       </c>
       <c r="I7">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>0.92088740058601948</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.45">
@@ -638,23 +635,23 @@
       </c>
       <c r="D8">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>85</v>
       </c>
       <c r="E8">
         <f t="shared" si="3"/>
-        <v>10</v>
+        <v>3624.2592592592596</v>
       </c>
       <c r="G8">
         <f t="shared" si="0"/>
-        <v>0.6</v>
+        <v>7.3241019876347652E-2</v>
       </c>
       <c r="H8">
         <f t="shared" si="0"/>
-        <v>0.6</v>
+        <v>0.29296407950539061</v>
       </c>
       <c r="I8">
         <f t="shared" si="0"/>
-        <v>0.6</v>
+        <v>0.97654693168463536</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.45">
@@ -668,23 +665,23 @@
       </c>
       <c r="D9">
         <f>C9+D8*D$4</f>
-        <v>5</v>
+        <v>341</v>
       </c>
       <c r="E9">
         <f t="shared" si="3"/>
-        <v>15</v>
+        <v>48664.456790123462</v>
       </c>
       <c r="G9">
         <f t="shared" si="0"/>
-        <v>0.66666666666666663</v>
+        <v>7.4474462437538386E-2</v>
       </c>
       <c r="H9">
         <f t="shared" si="0"/>
-        <v>0.66666666666666663</v>
+        <v>0.29789784975015354</v>
       </c>
       <c r="I9">
         <f t="shared" si="0"/>
-        <v>0.66666666666666663</v>
+        <v>0.99299283250051185</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.45">
@@ -698,28 +695,28 @@
       </c>
       <c r="D10">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>1365</v>
       </c>
       <c r="E10">
         <f t="shared" si="3"/>
-        <v>21</v>
+        <v>650224.42386831285</v>
       </c>
       <c r="G10">
         <f t="shared" si="0"/>
-        <v>0.7142857142857143</v>
+        <v>7.4842554360860583E-2</v>
       </c>
       <c r="H10">
         <f t="shared" si="0"/>
-        <v>0.7142857142857143</v>
+        <v>0.29937021744344233</v>
       </c>
       <c r="I10">
         <f t="shared" si="0"/>
-        <v>0.7142857142857143</v>
+        <v>0.99790072481147452</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B11">
-        <f t="shared" si="4"/>
+        <f>B10+1</f>
         <v>6</v>
       </c>
       <c r="C11">
@@ -728,23 +725,473 @@
       </c>
       <c r="D11">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>5461</v>
       </c>
       <c r="E11">
         <f>D11+E10*E$4</f>
-        <v>28</v>
+        <v>8675119.9849108383</v>
       </c>
       <c r="G11">
         <f t="shared" si="0"/>
-        <v>0.75</v>
+        <v>7.4952787396518727E-2</v>
       </c>
       <c r="H11">
         <f t="shared" si="0"/>
-        <v>0.75</v>
+        <v>0.29981114958607491</v>
       </c>
       <c r="I11">
         <f t="shared" si="0"/>
-        <v>0.75</v>
+        <v>0.99937049862024974</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B12">
+        <f t="shared" ref="B12:B26" si="5">B11+1</f>
+        <v>7</v>
+      </c>
+      <c r="C12">
+        <f t="shared" ref="C12:C22" si="6">POWER(C$4,B12)</f>
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <f t="shared" ref="D12:D22" si="7">C12+D11*D$4</f>
+        <v>21845</v>
+      </c>
+      <c r="E12">
+        <f t="shared" ref="E12:E22" si="8">D12+E11*E$4</f>
+        <v>115690111.46547785</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>7.4985838245125294E-2</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>0.29994335298050118</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="0"/>
+        <v>0.99981117660167063</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B13">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="7"/>
+        <v>87381</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="8"/>
+        <v>1542622200.5397048</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>7.4995751665574553E-2</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="0"/>
+        <v>0.29998300666229821</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="0"/>
+        <v>0.99994335554099412</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B14">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="7"/>
+        <v>349525</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="8"/>
+        <v>20568645532.196064</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>7.4998725517683745E-2</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>0.29999490207073498</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="0"/>
+        <v>0.99998300690245001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B15">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="7"/>
+        <v>1398101</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="8"/>
+        <v>274250005196.94754</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>7.4999617656980808E-2</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="0"/>
+        <v>0.29999847062792323</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="0"/>
+        <v>0.99999490209307751</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B16">
+        <f t="shared" si="5"/>
+        <v>11</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="7"/>
+        <v>5592405</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="8"/>
+        <v>3656672328364.3008</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>7.4999885297249144E-2</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="0"/>
+        <v>0.29999954118899658</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="0"/>
+        <v>0.99999847062998859</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B17">
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="7"/>
+        <v>22369621</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="8"/>
+        <v>48755653414478.344</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="0"/>
+        <v>7.4999965589188991E-2</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="0"/>
+        <v>0.29999986235675596</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="0"/>
+        <v>0.99999954118918655</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B18">
+        <f t="shared" si="5"/>
+        <v>13</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="7"/>
+        <v>89478485</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="8"/>
+        <v>650075468338196.25</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="0"/>
+        <v>7.4999989676758E-2</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="0"/>
+        <v>0.299999958707032</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="0"/>
+        <v>0.99999986235677341</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B19">
+        <f t="shared" si="5"/>
+        <v>14</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="7"/>
+        <v>357913941</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="8"/>
+        <v>8667673269089891</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="0"/>
+        <v>7.4999996903027527E-2</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="0"/>
+        <v>0.29999998761211011</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="0"/>
+        <v>0.99999995870703373</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B20">
+        <f t="shared" si="5"/>
+        <v>15</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="7"/>
+        <v>1431655765</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="8"/>
+        <v>1.155689783528543E+17</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="0"/>
+        <v>7.4999999070908277E-2</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="0"/>
+        <v>0.29999999628363311</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="0"/>
+        <v>0.9999999876121104</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B21">
+        <f t="shared" si="5"/>
+        <v>16</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="7"/>
+        <v>5726623061</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="8"/>
+        <v>1.5409197170980137E+18</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="0"/>
+        <v>7.4999999721272484E-2</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="0"/>
+        <v>0.29999999888508994</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="0"/>
+        <v>0.99999999628363312</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B22">
+        <f t="shared" si="5"/>
+        <v>17</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="7"/>
+        <v>22906492245</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="8"/>
+        <v>2.0545596250880008E+19</v>
+      </c>
+      <c r="G22">
+        <f t="shared" ref="G22:I26" si="9">C$4*($E21/$E22)</f>
+        <v>7.4999999916381746E-2</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="9"/>
+        <v>0.29999999966552698</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="9"/>
+        <v>0.99999999888508995</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B23">
+        <f t="shared" si="5"/>
+        <v>18</v>
+      </c>
+      <c r="C23">
+        <f t="shared" ref="C23:C26" si="10">POWER(C$4,B23)</f>
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <f t="shared" ref="D23:D26" si="11">C23+D22*D$4</f>
+        <v>91625968981</v>
+      </c>
+      <c r="E23">
+        <f t="shared" ref="E23:E26" si="12">D23+E22*E$4</f>
+        <v>2.7394128343669277E+20</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="9"/>
+        <v>7.4999999974914522E-2</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="9"/>
+        <v>0.29999999989965809</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="9"/>
+        <v>0.999999999665527</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B24">
+        <f t="shared" si="5"/>
+        <v>19</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="11"/>
+        <v>366503875925</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="12"/>
+        <v>3.6525504461890744E+21</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="9"/>
+        <v>7.499999999247435E-2</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="9"/>
+        <v>0.2999999999698974</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="9"/>
+        <v>0.99999999989965804</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B25">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="11"/>
+        <v>1466015503701</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="12"/>
+        <v>4.8700672617320347E+22</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="9"/>
+        <v>7.4999999997742303E-2</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="9"/>
+        <v>0.29999999999096921</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="9"/>
+        <v>0.99999999996989741</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B26">
+        <f t="shared" si="5"/>
+        <v>21</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="11"/>
+        <v>5864062014805</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="12"/>
+        <v>6.4934230157013542E+23</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="9"/>
+        <v>7.4999999999322678E-2</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="9"/>
+        <v>0.29999999999729071</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="9"/>
+        <v>0.99999999999096911</v>
       </c>
     </row>
   </sheetData>

</xml_diff>